<commit_message>
Completed SQL import script, extended user table to include forum flag
</commit_message>
<xml_diff>
--- a/sql/codesign_categories_ideas_etc.xlsx
+++ b/sql/codesign_categories_ideas_etc.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="204">
   <si>
     <t>Categories</t>
   </si>
@@ -668,6 +668,21 @@
   </si>
   <si>
     <t>File</t>
+  </si>
+  <si>
+    <t>INSERT INTO `codesign_production`.`project` (`id`, `category_id`, `incubated`, `hidden`, `name`, `overview`, `description`) VALUES ({PROJECT_ID}, {CATEGORY_ID}, 1, 0, '{TITLE}', '{OVERVIEW}', '{DESCRIPTION}');</t>
+  </si>
+  <si>
+    <t>INSERT INTO `codesign_production`.`idea_project` (`idea_id`, `project_id`) VALUES ({IDEA_ID}, {PROJECT_ID});</t>
+  </si>
+  <si>
+    <t>IdeaID</t>
+  </si>
+  <si>
+    <t>Project_ID</t>
+  </si>
+  <si>
+    <t>INSERT INTO `codesign_production`.`project` (`id`, `category_id`, `incubated`, `hidden`, `name`, `overview`, `description`) VALUES ({PROJECT_ID}, {CATEGORY_ID}, 0, 0, '{TITLE}', '{OVERVIEW}', '{DESCRIPTION}');</t>
   </si>
 </sst>
 </file>
@@ -761,9 +776,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -793,11 +818,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="16">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1098,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N74"/>
+  <dimension ref="A1:P77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="N72" sqref="N72:P77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1109,6 +1144,7 @@
     <col min="6" max="6" width="11.33203125" customWidth="1"/>
     <col min="10" max="10" width="15.83203125" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="14" max="14" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -2134,12 +2170,34 @@
         <v>INSERT INTO `codesign_production`.`idea` (`id`, `user_id`, `category_id`, `title`, `overview`, `description`) VALUES (35, 1, 3, 'Report and practical guide to preparing costs for RDM services.', 'Making it easier to prepare cost estimates for managing research data', 'One of the first – if not THE first – questions of senior management considering institutional RDM services is ‘how much will it cost’?  Unfortunately, this question is not easy to answer as it relates to an evolving activity for which there is limited prior art.  This study will be a first step to systematising knowledge and predictions of costs, based squarely on existing practices in universities.  The output will be a first edition of a practical guide to preparing cost estimates for various components of RDM services.');</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:16">
       <c r="A53" t="s">
+        <v>201</v>
+      </c>
+      <c r="B53" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="F53" t="s">
+        <v>195</v>
+      </c>
+      <c r="G53" t="s">
+        <v>202</v>
+      </c>
+      <c r="N53" s="9" t="str">
+        <f>N13</f>
+        <v>INSERT INTO `codesign_production`.`idea` (`id`, `user_id`, `category_id`, `title`, `overview`, `description`) VALUES ({ID}, 1, {CATEGORY_ID}, '{TITLE}', '{OVERVIEW}', '{DESCRIPTION}');</v>
+      </c>
+      <c r="O53" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="P53" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16">
+      <c r="A54">
+        <v>36</v>
+      </c>
       <c r="B54" s="1" t="s">
         <v>51</v>
       </c>
@@ -2152,8 +2210,30 @@
       <c r="E54" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="F54">
+        <f>VLOOKUP(E54,$B$3:$C$6,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="N54" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($N$53,"{ID}",A54), "{CATEGORY_ID}",F54),"{TITLE}",B54),"{OVERVIEW}",C54), "{DESCRIPTION}",D54)</f>
+        <v>INSERT INTO `codesign_production`.`idea` (`id`, `user_id`, `category_id`, `title`, `overview`, `description`) VALUES (36, 1, 3, 'Data Governance', 'Looking at the big picture of data management within universities', 'Universities need to manage a range of different types of data. Each of these have their own requirements and drivers. Universities need to be confident that they are managing each data type according to its specific demands while ensuring that the data can be reused to serve research, teaching and wealth creation missions. This project will look at that big picture and seek to identify what can be done to support universities in pursuing robust data management');</v>
+      </c>
+      <c r="O54" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($O$53,"{IDEA_ID}",A54), "{CATEGORY_ID}",F54),"{TITLE}",B54),"{OVERVIEW}",C54), "{DESCRIPTION}",D54),"{PROJECT_ID}",G54)</f>
+        <v>INSERT INTO `codesign_production`.`project` (`id`, `category_id`, `incubated`, `hidden`, `name`, `overview`, `description`) VALUES (1, 3, 1, 0, 'Data Governance', 'Looking at the big picture of data management within universities', 'Universities need to manage a range of different types of data. Each of these have their own requirements and drivers. Universities need to be confident that they are managing each data type according to its specific demands while ensuring that the data can be reused to serve research, teaching and wealth creation missions. This project will look at that big picture and seek to identify what can be done to support universities in pursuing robust data management');</v>
+      </c>
+      <c r="P54" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE($P$53,"{IDEA_ID}",A54),"{PROJECT_ID}",G54)</f>
+        <v>INSERT INTO `codesign_production`.`idea_project` (`idea_id`, `project_id`) VALUES (36, 1);</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16">
+      <c r="A55">
+        <v>37</v>
+      </c>
       <c r="B55" s="1" t="s">
         <v>52</v>
       </c>
@@ -2166,8 +2246,30 @@
       <c r="E55" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="F55">
+        <f t="shared" ref="F55:F67" si="2">VLOOKUP(E55,$B$3:$C$6,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="G55">
+        <v>2</v>
+      </c>
+      <c r="N55" t="str">
+        <f t="shared" ref="N55:N67" si="3">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($N$53,"{ID}",A55), "{CATEGORY_ID}",F55),"{TITLE}",B55),"{OVERVIEW}",C55), "{DESCRIPTION}",D55)</f>
+        <v>INSERT INTO `codesign_production`.`idea` (`id`, `user_id`, `category_id`, `title`, `overview`, `description`) VALUES (37, 1, 3, 'Innovation Case Studies', 'Identifying innovation good practice that universities could use to create a productive environment for innovation', 'Universities need to innovate to succeed but are faced with limited resources and time and some institutions are unsure of the most effective approaches to take to innovate. Jisc, SCONUL, RLUK, RUGIT and UCISA are undertaking some innovation on behalf of the sector and want to ensure that this innovation is informed by good ideas from outside the sector. This is a short piece of work to produce some compelling case studies that can help universities and the co-designers in designing innovation approaches.');</v>
+      </c>
+      <c r="O55" t="str">
+        <f t="shared" ref="O55:O67" si="4">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($O$53,"{IDEA_ID}",A55), "{CATEGORY_ID}",F55),"{TITLE}",B55),"{OVERVIEW}",C55), "{DESCRIPTION}",D55),"{PROJECT_ID}",G55)</f>
+        <v>INSERT INTO `codesign_production`.`project` (`id`, `category_id`, `incubated`, `hidden`, `name`, `overview`, `description`) VALUES (2, 3, 1, 0, 'Innovation Case Studies', 'Identifying innovation good practice that universities could use to create a productive environment for innovation', 'Universities need to innovate to succeed but are faced with limited resources and time and some institutions are unsure of the most effective approaches to take to innovate. Jisc, SCONUL, RLUK, RUGIT and UCISA are undertaking some innovation on behalf of the sector and want to ensure that this innovation is informed by good ideas from outside the sector. This is a short piece of work to produce some compelling case studies that can help universities and the co-designers in designing innovation approaches.');</v>
+      </c>
+      <c r="P55" t="str">
+        <f t="shared" ref="P55:P67" si="5">SUBSTITUTE(SUBSTITUTE($P$53,"{IDEA_ID}",A55),"{PROJECT_ID}",G55)</f>
+        <v>INSERT INTO `codesign_production`.`idea_project` (`idea_id`, `project_id`) VALUES (37, 2);</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16">
+      <c r="A56">
+        <v>38</v>
+      </c>
       <c r="B56" s="1" t="s">
         <v>53</v>
       </c>
@@ -2180,8 +2282,30 @@
       <c r="E56" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="F56">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G56">
+        <v>3</v>
+      </c>
+      <c r="N56" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `codesign_production`.`idea` (`id`, `user_id`, `category_id`, `title`, `overview`, `description`) VALUES (38, 1, 2, 'Issues with Shared Infrastructure', 'Exploring what would help universities benefit from cloud and shared service opportunities?', 'Cloud and shared infrastructure services present opportunities for universities to provide more efficient services. However uptake of these services has not been as widespread as they might have been. This project would seek to find out why and to identify any support that can be offered to allow university IT managers to seize on opportunities presented by the cloud and shared infrastructure. ');</v>
+      </c>
+      <c r="O56" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO `codesign_production`.`project` (`id`, `category_id`, `incubated`, `hidden`, `name`, `overview`, `description`) VALUES (3, 2, 1, 0, 'Issues with Shared Infrastructure', 'Exploring what would help universities benefit from cloud and shared service opportunities?', 'Cloud and shared infrastructure services present opportunities for universities to provide more efficient services. However uptake of these services has not been as widespread as they might have been. This project would seek to find out why and to identify any support that can be offered to allow university IT managers to seize on opportunities presented by the cloud and shared infrastructure. ');</v>
+      </c>
+      <c r="P56" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO `codesign_production`.`idea_project` (`idea_id`, `project_id`) VALUES (38, 3);</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16">
+      <c r="A57">
+        <v>39</v>
+      </c>
       <c r="B57" s="1" t="s">
         <v>62</v>
       </c>
@@ -2194,8 +2318,30 @@
       <c r="E57" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="F57">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="G57">
+        <v>4</v>
+      </c>
+      <c r="N57" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `codesign_production`.`idea` (`id`, `user_id`, `category_id`, `title`, `overview`, `description`) VALUES (39, 1, 3, 'Analytics - scenario planning', 'Using data and analytics to support a responsive approach to planning in universities', 'Universities need to adopt more responsive methods of corporate planning due to the new funding regime. They are having to respond quickly to changes in student intake numbers and the resulting adjustment to fees. Analytics could help universities plan for a range of different scenarios to enable them to be more responsive in the way that they operate. This project will explore this opportunity and identify actions that could benefit institutions and the sector as a whole.  ');</v>
+      </c>
+      <c r="O57" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO `codesign_production`.`project` (`id`, `category_id`, `incubated`, `hidden`, `name`, `overview`, `description`) VALUES (4, 3, 1, 0, 'Analytics - scenario planning', 'Using data and analytics to support a responsive approach to planning in universities', 'Universities need to adopt more responsive methods of corporate planning due to the new funding regime. They are having to respond quickly to changes in student intake numbers and the resulting adjustment to fees. Analytics could help universities plan for a range of different scenarios to enable them to be more responsive in the way that they operate. This project will explore this opportunity and identify actions that could benefit institutions and the sector as a whole.  ');</v>
+      </c>
+      <c r="P57" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO `codesign_production`.`idea_project` (`idea_id`, `project_id`) VALUES (39, 4);</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16">
+      <c r="A58">
+        <v>40</v>
+      </c>
       <c r="B58" s="1" t="s">
         <v>30</v>
       </c>
@@ -2208,8 +2354,30 @@
       <c r="E58" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="F58">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G58">
+        <v>5</v>
+      </c>
+      <c r="N58" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `codesign_production`.`idea` (`id`, `user_id`, `category_id`, `title`, `overview`, `description`) VALUES (40, 1, 2, 'Shared Resilience', 'Exploring what could be learned from the YHMAN project', 'YHMAN is a project that links universities in the Yorkshire and Humber area through a shared infrastructure. This potentially offers a shared infrastructure model that could be relevant elsewhere in the UK. This project would take YHMAN knowledge and make it usable for other institutions');</v>
+      </c>
+      <c r="O58" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO `codesign_production`.`project` (`id`, `category_id`, `incubated`, `hidden`, `name`, `overview`, `description`) VALUES (5, 2, 1, 0, 'Shared Resilience', 'Exploring what could be learned from the YHMAN project', 'YHMAN is a project that links universities in the Yorkshire and Humber area through a shared infrastructure. This potentially offers a shared infrastructure model that could be relevant elsewhere in the UK. This project would take YHMAN knowledge and make it usable for other institutions');</v>
+      </c>
+      <c r="P58" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO `codesign_production`.`idea_project` (`idea_id`, `project_id`) VALUES (40, 5);</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16">
+      <c r="A59">
+        <v>41</v>
+      </c>
       <c r="B59" s="1" t="s">
         <v>54</v>
       </c>
@@ -2222,8 +2390,30 @@
       <c r="E59" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="F59">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="G59">
+        <v>6</v>
+      </c>
+      <c r="N59" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `codesign_production`.`idea` (`id`, `user_id`, `category_id`, `title`, `overview`, `description`) VALUES (41, 1, 3, 'Bring Your Own Device', 'Supporting students and staff in using their own computing devices to access university services', 'Students and staff often want to use their personal computing devices instead of university supplied devices. This is something that many universities are already dealing with. This work would combine research into the challenges that BYOD brings with the development of a toolkit that shares good practice in this area and provides universities with template policies, business case information etc that they can use to help their planning and implementation of BYOD.');</v>
+      </c>
+      <c r="O59" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO `codesign_production`.`project` (`id`, `category_id`, `incubated`, `hidden`, `name`, `overview`, `description`) VALUES (6, 3, 1, 0, 'Bring Your Own Device', 'Supporting students and staff in using their own computing devices to access university services', 'Students and staff often want to use their personal computing devices instead of university supplied devices. This is something that many universities are already dealing with. This work would combine research into the challenges that BYOD brings with the development of a toolkit that shares good practice in this area and provides universities with template policies, business case information etc that they can use to help their planning and implementation of BYOD.');</v>
+      </c>
+      <c r="P59" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO `codesign_production`.`idea_project` (`idea_id`, `project_id`) VALUES (41, 6);</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16">
+      <c r="A60">
+        <v>42</v>
+      </c>
       <c r="B60" s="1" t="s">
         <v>55</v>
       </c>
@@ -2236,8 +2426,30 @@
       <c r="E60" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="F60">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="G60">
+        <v>7</v>
+      </c>
+      <c r="N60" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `codesign_production`.`idea` (`id`, `user_id`, `category_id`, `title`, `overview`, `description`) VALUES (42, 1, 4, 'High Performance Computing', 'Are there services that could be provided to make high performance computing easier to use?', 'High performance computing is used throughout HE. However barriers to using it are quite high and there is the possibility that more people could benefit from using it in their research if it were easier to use.');</v>
+      </c>
+      <c r="O60" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO `codesign_production`.`project` (`id`, `category_id`, `incubated`, `hidden`, `name`, `overview`, `description`) VALUES (7, 4, 1, 0, 'High Performance Computing', 'Are there services that could be provided to make high performance computing easier to use?', 'High performance computing is used throughout HE. However barriers to using it are quite high and there is the possibility that more people could benefit from using it in their research if it were easier to use.');</v>
+      </c>
+      <c r="P60" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO `codesign_production`.`idea_project` (`idea_id`, `project_id`) VALUES (42, 7);</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16">
+      <c r="A61">
+        <v>43</v>
+      </c>
       <c r="B61" s="1" t="s">
         <v>56</v>
       </c>
@@ -2250,8 +2462,30 @@
       <c r="E61" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="62" spans="1:5">
+      <c r="F61">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G61">
+        <v>8</v>
+      </c>
+      <c r="N61" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `codesign_production`.`idea` (`id`, `user_id`, `category_id`, `title`, `overview`, `description`) VALUES (43, 1, 2, 'Shared Research Data Suite', 'Developing a proposition for a research data management infrastructure', 'Many UK universities are facing drivers from the research councils and government to set up robust research data management processes. There is not an obvious solution that can satisfy these demands. This piece of work would examine the issues involved in institutional research data management and seek to articulate a proposition for how research data management infrastructure can address research requirements in the UK and meet the demands of the research council. ');</v>
+      </c>
+      <c r="O61" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO `codesign_production`.`project` (`id`, `category_id`, `incubated`, `hidden`, `name`, `overview`, `description`) VALUES (8, 2, 1, 0, 'Shared Research Data Suite', 'Developing a proposition for a research data management infrastructure', 'Many UK universities are facing drivers from the research councils and government to set up robust research data management processes. There is not an obvious solution that can satisfy these demands. This piece of work would examine the issues involved in institutional research data management and seek to articulate a proposition for how research data management infrastructure can address research requirements in the UK and meet the demands of the research council. ');</v>
+      </c>
+      <c r="P61" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO `codesign_production`.`idea_project` (`idea_id`, `project_id`) VALUES (43, 8);</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16">
+      <c r="A62">
+        <v>44</v>
+      </c>
       <c r="B62" s="1" t="s">
         <v>57</v>
       </c>
@@ -2264,8 +2498,30 @@
       <c r="E62" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="63" spans="1:5">
+      <c r="F62">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="G62">
+        <v>9</v>
+      </c>
+      <c r="N62" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `codesign_production`.`idea` (`id`, `user_id`, `category_id`, `title`, `overview`, `description`) VALUES (44, 1, 3, 'Collecting the UK Web', 'Exploring how electronic legal deposit can benefit researchers', 'After many years of waiting, the UK now has structures in place that allow our national libraries to collect legal deposit material electronically and to harvest and archive the web.  We do not yet have clear collection management policies that reflect our view of the needs of future researchers - in the short, medium and long term.');</v>
+      </c>
+      <c r="O62" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO `codesign_production`.`project` (`id`, `category_id`, `incubated`, `hidden`, `name`, `overview`, `description`) VALUES (9, 3, 1, 0, 'Collecting the UK Web', 'Exploring how electronic legal deposit can benefit researchers', 'After many years of waiting, the UK now has structures in place that allow our national libraries to collect legal deposit material electronically and to harvest and archive the web.  We do not yet have clear collection management policies that reflect our view of the needs of future researchers - in the short, medium and long term.');</v>
+      </c>
+      <c r="P62" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO `codesign_production`.`idea_project` (`idea_id`, `project_id`) VALUES (44, 9);</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16">
+      <c r="A63">
+        <v>45</v>
+      </c>
       <c r="B63" s="1" t="s">
         <v>60</v>
       </c>
@@ -2278,8 +2534,30 @@
       <c r="E63" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="64" spans="1:5">
+      <c r="F63">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G63">
+        <v>10</v>
+      </c>
+      <c r="N63" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `codesign_production`.`idea` (`id`, `user_id`, `category_id`, `title`, `overview`, `description`) VALUES (45, 1, 2, 'Document supply', 'Identifying new approaches to document supply', 'This idea will focus on examining the current document supply approaches used by libraries and then identifying possible new approaches. These new approaches will be analysed to determine possible benefits and prototypes will be built of the most promising options. ');</v>
+      </c>
+      <c r="O63" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO `codesign_production`.`project` (`id`, `category_id`, `incubated`, `hidden`, `name`, `overview`, `description`) VALUES (10, 2, 1, 0, 'Document supply', 'Identifying new approaches to document supply', 'This idea will focus on examining the current document supply approaches used by libraries and then identifying possible new approaches. These new approaches will be analysed to determine possible benefits and prototypes will be built of the most promising options. ');</v>
+      </c>
+      <c r="P63" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO `codesign_production`.`idea_project` (`idea_id`, `project_id`) VALUES (45, 10);</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16">
+      <c r="A64">
+        <v>46</v>
+      </c>
       <c r="B64" s="1" t="s">
         <v>58</v>
       </c>
@@ -2292,8 +2570,30 @@
       <c r="E64" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="65" spans="1:5">
+      <c r="F64">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G64">
+        <v>11</v>
+      </c>
+      <c r="N64" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `codesign_production`.`idea` (`id`, `user_id`, `category_id`, `title`, `overview`, `description`) VALUES (46, 1, 1, 'UK linked national catalogue', 'Releasing the Copac catalogue  as linked data', 'There is currently no integrated catalogue for UK FHE holdings.  This project would form the basis of that catalogue by releasing COPAC catalogue records in linked data format.  The records would be free to download and would allow for the development of new and innovative services, particularly in the areas of discoverability and access');</v>
+      </c>
+      <c r="O64" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO `codesign_production`.`project` (`id`, `category_id`, `incubated`, `hidden`, `name`, `overview`, `description`) VALUES (11, 1, 1, 0, 'UK linked national catalogue', 'Releasing the Copac catalogue  as linked data', 'There is currently no integrated catalogue for UK FHE holdings.  This project would form the basis of that catalogue by releasing COPAC catalogue records in linked data format.  The records would be free to download and would allow for the development of new and innovative services, particularly in the areas of discoverability and access');</v>
+      </c>
+      <c r="P64" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO `codesign_production`.`idea_project` (`idea_id`, `project_id`) VALUES (46, 11);</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16">
+      <c r="A65">
+        <v>47</v>
+      </c>
       <c r="B65" s="1" t="s">
         <v>59</v>
       </c>
@@ -2306,8 +2606,30 @@
       <c r="E65" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="66" spans="1:5">
+      <c r="F65">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="G65">
+        <v>12</v>
+      </c>
+      <c r="N65" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `codesign_production`.`idea` (`id`, `user_id`, `category_id`, `title`, `overview`, `description`) VALUES (47, 1, 3, 'Research data', 'Developing a roadmap for research data activity', 'Many UK universities are facing drivers from the research councils and government to set up robust research data management processes. There is a lot of work occurring to meet these drivers. This piece of work would take a strategic view of the UK’s research data activities and seek to create a roadmap for future activity.');</v>
+      </c>
+      <c r="O65" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO `codesign_production`.`project` (`id`, `category_id`, `incubated`, `hidden`, `name`, `overview`, `description`) VALUES (12, 3, 1, 0, 'Research data', 'Developing a roadmap for research data activity', 'Many UK universities are facing drivers from the research councils and government to set up robust research data management processes. There is a lot of work occurring to meet these drivers. This piece of work would take a strategic view of the UK’s research data activities and seek to create a roadmap for future activity.');</v>
+      </c>
+      <c r="P65" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO `codesign_production`.`idea_project` (`idea_id`, `project_id`) VALUES (47, 12);</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16">
+      <c r="A66">
+        <v>48</v>
+      </c>
       <c r="B66" s="1" t="s">
         <v>61</v>
       </c>
@@ -2320,8 +2642,30 @@
       <c r="E66" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="67" spans="1:5">
+      <c r="F66">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="G66">
+        <v>13</v>
+      </c>
+      <c r="N66" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `codesign_production`.`idea` (`id`, `user_id`, `category_id`, `title`, `overview`, `description`) VALUES (48, 1, 4, 'The Digital Student', 'Studying the digital requirements of students about to enter universities', 'Students are entering university with very different expectations and requirements for a digital experience than past students or university staff. This is driven by developments in mobile technology and by web trends. Universities may need help in establishing a detailed understanding of these requirements to enable them to tweak or reimagine the services they offer.  ');</v>
+      </c>
+      <c r="O66" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO `codesign_production`.`project` (`id`, `category_id`, `incubated`, `hidden`, `name`, `overview`, `description`) VALUES (13, 4, 1, 0, 'The Digital Student', 'Studying the digital requirements of students about to enter universities', 'Students are entering university with very different expectations and requirements for a digital experience than past students or university staff. This is driven by developments in mobile technology and by web trends. Universities may need help in establishing a detailed understanding of these requirements to enable them to tweak or reimagine the services they offer.  ');</v>
+      </c>
+      <c r="P66" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO `codesign_production`.`idea_project` (`idea_id`, `project_id`) VALUES (48, 13);</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16">
+      <c r="A67">
+        <v>49</v>
+      </c>
       <c r="B67" s="1" t="s">
         <v>63</v>
       </c>
@@ -2334,99 +2678,256 @@
       <c r="E67" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="68" spans="1:5">
-      <c r="A68" t="s">
+      <c r="F67">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="G67">
+        <v>14</v>
+      </c>
+      <c r="N67" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO `codesign_production`.`idea` (`id`, `user_id`, `category_id`, `title`, `overview`, `description`) VALUES (49, 1, 4, 'Analytics - student journey', 'Can analytics be used to provide students with new tools to choose what and how to study', 'New approaches to analytics potentially offer benefits to higher education in helping students make choices about their education. However there is currently not a clear picture of what the opportunities are, nor is it clear who is ready to take those opportunities. This project would seek to develop a vision for how students could benefit from analytics, develop tools to encourage action and seek opportunities to develop services to help UKHE realise benefits. ');</v>
+      </c>
+      <c r="O67" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO `codesign_production`.`project` (`id`, `category_id`, `incubated`, `hidden`, `name`, `overview`, `description`) VALUES (14, 4, 1, 0, 'Analytics - student journey', 'Can analytics be used to provide students with new tools to choose what and how to study', 'New approaches to analytics potentially offer benefits to higher education in helping students make choices about their education. However there is currently not a clear picture of what the opportunities are, nor is it clear who is ready to take those opportunities. This project would seek to develop a vision for how students could benefit from analytics, develop tools to encourage action and seek opportunities to develop services to help UKHE realise benefits. ');</v>
+      </c>
+      <c r="P67" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO `codesign_production`.`idea_project` (`idea_id`, `project_id`) VALUES (49, 14);</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16">
+      <c r="A71" t="s">
+        <v>201</v>
+      </c>
+      <c r="B71" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="69" spans="1:5">
-      <c r="B69" t="s">
+      <c r="O71" s="9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16">
+      <c r="A72">
+        <v>50</v>
+      </c>
+      <c r="B72" t="s">
         <v>14</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C72" t="s">
         <v>173</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D72" t="s">
         <v>20</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E72" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="B70" t="s">
+      <c r="F72">
+        <f t="shared" ref="F72:F77" si="6">VLOOKUP(E72,$B$3:$C$6,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="G72">
         <v>15</v>
       </c>
-      <c r="C70" t="s">
+      <c r="N72" t="str">
+        <f t="shared" ref="N72" si="7">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($N$53,"{ID}",A72), "{CATEGORY_ID}",F72),"{TITLE}",B72),"{OVERVIEW}",C72), "{DESCRIPTION}",D72)</f>
+        <v>INSERT INTO `codesign_production`.`idea` (`id`, `user_id`, `category_id`, `title`, `overview`, `description`) VALUES (50, 1, 1, 'Green Mirror', 'Exploring how we can make more of the open access material published by UK authors', 'UK authors publish over 100,000 peer-reviewed papers each year.  These are scattered across thousands of journals and repositories.  With funder-driven mandates requiring that research outputs be made open access we have the opportunity to bring these papers together to demonstrate the UK’s intellectual wealth.  Doing so would make these outputs more discoverable, encourage researchers to deposit in local repositories and could potentially aid long-term preservation and facilitate text and data mining ');</v>
+      </c>
+      <c r="O72" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($O$71,"{IDEA_ID}",A72), "{CATEGORY_ID}",F72),"{TITLE}",B72),"{OVERVIEW}",C72), "{DESCRIPTION}",D72),"{PROJECT_ID}",G72)</f>
+        <v>INSERT INTO `codesign_production`.`project` (`id`, `category_id`, `incubated`, `hidden`, `name`, `overview`, `description`) VALUES (15, 1, 0, 0, 'Green Mirror', 'Exploring how we can make more of the open access material published by UK authors', 'UK authors publish over 100,000 peer-reviewed papers each year.  These are scattered across thousands of journals and repositories.  With funder-driven mandates requiring that research outputs be made open access we have the opportunity to bring these papers together to demonstrate the UK’s intellectual wealth.  Doing so would make these outputs more discoverable, encourage researchers to deposit in local repositories and could potentially aid long-term preservation and facilitate text and data mining ');</v>
+      </c>
+      <c r="P72" t="str">
+        <f t="shared" ref="P72" si="8">SUBSTITUTE(SUBSTITUTE($P$53,"{IDEA_ID}",A72),"{PROJECT_ID}",G72)</f>
+        <v>INSERT INTO `codesign_production`.`idea_project` (`idea_id`, `project_id`) VALUES (50, 15);</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16">
+      <c r="A73">
+        <v>51</v>
+      </c>
+      <c r="B73" t="s">
+        <v>15</v>
+      </c>
+      <c r="C73" t="s">
         <v>174</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="D73" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E73" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="71" spans="1:5">
-      <c r="B71" t="s">
+      <c r="F73">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="G73">
         <v>16</v>
       </c>
-      <c r="C71" t="s">
+      <c r="N73" t="str">
+        <f t="shared" ref="N73:N78" si="9">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($N$53,"{ID}",A73), "{CATEGORY_ID}",F73),"{TITLE}",B73),"{OVERVIEW}",C73), "{DESCRIPTION}",D73)</f>
+        <v>INSERT INTO `codesign_production`.`idea` (`id`, `user_id`, `category_id`, `title`, `overview`, `description`) VALUES (51, 1, 1, 'Spotlight on the Digital', 'Exploring how we can make more of the digitised content released by UK universities', 'While there have been a great many digitisation projects over the past two decades, it is not clear that the digitised outputs are as discoverable as they should be, leading to less usage by researchers.  We have created a series of islands of content that are not cross-searchable or capable of being integrated.  This work would look to rectify this and ensure that future digitisation projects address the discoverability issue from the start. ');</v>
+      </c>
+      <c r="O73" t="str">
+        <f t="shared" ref="O73:O78" si="10">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($O$71,"{IDEA_ID}",A73), "{CATEGORY_ID}",F73),"{TITLE}",B73),"{OVERVIEW}",C73), "{DESCRIPTION}",D73),"{PROJECT_ID}",G73)</f>
+        <v>INSERT INTO `codesign_production`.`project` (`id`, `category_id`, `incubated`, `hidden`, `name`, `overview`, `description`) VALUES (16, 1, 0, 0, 'Spotlight on the Digital', 'Exploring how we can make more of the digitised content released by UK universities', 'While there have been a great many digitisation projects over the past two decades, it is not clear that the digitised outputs are as discoverable as they should be, leading to less usage by researchers.  We have created a series of islands of content that are not cross-searchable or capable of being integrated.  This work would look to rectify this and ensure that future digitisation projects address the discoverability issue from the start. ');</v>
+      </c>
+      <c r="P73" t="str">
+        <f t="shared" ref="P73:P78" si="11">SUBSTITUTE(SUBSTITUTE($P$53,"{IDEA_ID}",A73),"{PROJECT_ID}",G73)</f>
+        <v>INSERT INTO `codesign_production`.`idea_project` (`idea_id`, `project_id`) VALUES (51, 16);</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16">
+      <c r="A74">
+        <v>52</v>
+      </c>
+      <c r="B74" t="s">
+        <v>16</v>
+      </c>
+      <c r="C74" t="s">
         <v>175</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D74" t="s">
         <v>75</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E74" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="72" spans="1:5">
-      <c r="B72" t="s">
+      <c r="F74">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="G74">
         <v>17</v>
       </c>
-      <c r="C72" t="s">
+      <c r="N74" t="str">
+        <f t="shared" si="9"/>
+        <v>INSERT INTO `codesign_production`.`idea` (`id`, `user_id`, `category_id`, `title`, `overview`, `description`) VALUES (52, 1, 2, 'Extending Knowledge Base +', 'Developing Knowledge Base + to include e-book and post cancellation access data', 'KB+ has been developed to help libraries manage their electronic journal subscriptions more easily. The same approach and platform could be used to help libraries manage their e-book subscriptions and post cancellation access rights. This project would investigate the extension of KB+ to include information about e-book subscriptions and post cancellation access conditions');</v>
+      </c>
+      <c r="O74" t="str">
+        <f t="shared" si="10"/>
+        <v>INSERT INTO `codesign_production`.`project` (`id`, `category_id`, `incubated`, `hidden`, `name`, `overview`, `description`) VALUES (17, 2, 0, 0, 'Extending Knowledge Base +', 'Developing Knowledge Base + to include e-book and post cancellation access data', 'KB+ has been developed to help libraries manage their electronic journal subscriptions more easily. The same approach and platform could be used to help libraries manage their e-book subscriptions and post cancellation access rights. This project would investigate the extension of KB+ to include information about e-book subscriptions and post cancellation access conditions');</v>
+      </c>
+      <c r="P74" t="str">
+        <f t="shared" si="11"/>
+        <v>INSERT INTO `codesign_production`.`idea_project` (`idea_id`, `project_id`) VALUES (52, 17);</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16">
+      <c r="A75">
+        <v>53</v>
+      </c>
+      <c r="B75" t="s">
+        <v>17</v>
+      </c>
+      <c r="C75" t="s">
         <v>176</v>
       </c>
-      <c r="D72" s="3" t="s">
+      <c r="D75" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E75" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="73" spans="1:5">
-      <c r="B73" t="s">
+      <c r="F75">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="G75">
         <v>18</v>
       </c>
-      <c r="C73" t="s">
+      <c r="N75" t="str">
+        <f t="shared" si="9"/>
+        <v>INSERT INTO `codesign_production`.`idea` (`id`, `user_id`, `category_id`, `title`, `overview`, `description`) VALUES (53, 1, 3, 'National Monograph Strategy', 'Exploring a strategic approach to managing the monographs held by UK university libraries', 'Monograph collections have grown up based on local needs with no real national strategic focus.  As print collections age the community needs to make decisions on what should be preserved, what digitised (if not already) and what deaccessioned.  A national approach to this, exploiting technological solutions would encourage a shared service approach to maintaining access to print and to support the national needs of researchers. The value of this is recognised, and it must be part of a UK-wide strategic framework.  Aspects of the framework would include preservation strategies, priorities for digitisation (and an understanding of digital surrogates), discoverability issues and the role of document delivery services now and in the future');</v>
+      </c>
+      <c r="O75" t="str">
+        <f t="shared" si="10"/>
+        <v>INSERT INTO `codesign_production`.`project` (`id`, `category_id`, `incubated`, `hidden`, `name`, `overview`, `description`) VALUES (18, 3, 0, 0, 'National Monograph Strategy', 'Exploring a strategic approach to managing the monographs held by UK university libraries', 'Monograph collections have grown up based on local needs with no real national strategic focus.  As print collections age the community needs to make decisions on what should be preserved, what digitised (if not already) and what deaccessioned.  A national approach to this, exploiting technological solutions would encourage a shared service approach to maintaining access to print and to support the national needs of researchers. The value of this is recognised, and it must be part of a UK-wide strategic framework.  Aspects of the framework would include preservation strategies, priorities for digitisation (and an understanding of digital surrogates), discoverability issues and the role of document delivery services now and in the future');</v>
+      </c>
+      <c r="P75" t="str">
+        <f t="shared" si="11"/>
+        <v>INSERT INTO `codesign_production`.`idea_project` (`idea_id`, `project_id`) VALUES (53, 18);</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16">
+      <c r="A76">
+        <v>54</v>
+      </c>
+      <c r="B76" t="s">
+        <v>18</v>
+      </c>
+      <c r="C76" t="s">
         <v>177</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D76" t="s">
         <v>76</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E76" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="74" spans="1:5">
-      <c r="B74" t="s">
+      <c r="F76">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="G76">
         <v>19</v>
       </c>
-      <c r="C74" t="s">
+      <c r="N76" t="str">
+        <f t="shared" si="9"/>
+        <v>INSERT INTO `codesign_production`.`idea` (`id`, `user_id`, `category_id`, `title`, `overview`, `description`) VALUES (54, 1, 4, 'Identity Management', 'A focus on the cultural and political issues that univerisites face in administering identity management systems', 'This is an investigation into the cultural, social and political issues that are preventing excellent identity management in institutions. This investigation will explore the issue from a user’s point of view and will identify practical options for addressing the barriers identified. This project will take a library focus. ');</v>
+      </c>
+      <c r="O76" t="str">
+        <f t="shared" si="10"/>
+        <v>INSERT INTO `codesign_production`.`project` (`id`, `category_id`, `incubated`, `hidden`, `name`, `overview`, `description`) VALUES (19, 4, 0, 0, 'Identity Management', 'A focus on the cultural and political issues that univerisites face in administering identity management systems', 'This is an investigation into the cultural, social and political issues that are preventing excellent identity management in institutions. This investigation will explore the issue from a user’s point of view and will identify practical options for addressing the barriers identified. This project will take a library focus. ');</v>
+      </c>
+      <c r="P76" t="str">
+        <f t="shared" si="11"/>
+        <v>INSERT INTO `codesign_production`.`idea_project` (`idea_id`, `project_id`) VALUES (54, 19);</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16">
+      <c r="A77">
+        <v>55</v>
+      </c>
+      <c r="B77" t="s">
+        <v>19</v>
+      </c>
+      <c r="C77" t="s">
         <v>178</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="D77" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E77" t="s">
         <v>179</v>
       </c>
+      <c r="F77">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="G77">
+        <v>20</v>
+      </c>
+      <c r="N77" t="str">
+        <f t="shared" si="9"/>
+        <v>INSERT INTO `codesign_production`.`idea` (`id`, `user_id`, `category_id`, `title`, `overview`, `description`) VALUES (55, 1, 4, 'Student Innovation Teams', 'Funding teams of students to develop new technology to improve the student experience', 'This idea will put the power to innovate directly into the hands of teams of students, academics and experts by creating a paid summer programme for developing innovative technology. The teams will be selected through an open call for ideas. The technology developed by the teams will be embedded for a trial period in volunteer universities. Products that are successful in the trials will be provided to other interested parties through sustainable routes.');</v>
+      </c>
+      <c r="O77" t="str">
+        <f t="shared" si="10"/>
+        <v>INSERT INTO `codesign_production`.`project` (`id`, `category_id`, `incubated`, `hidden`, `name`, `overview`, `description`) VALUES (20, 4, 0, 0, 'Student Innovation Teams', 'Funding teams of students to develop new technology to improve the student experience', 'This idea will put the power to innovate directly into the hands of teams of students, academics and experts by creating a paid summer programme for developing innovative technology. The teams will be selected through an open call for ideas. The technology developed by the teams will be embedded for a trial period in volunteer universities. Products that are successful in the trials will be provided to other interested parties through sustainable routes.');</v>
+      </c>
+      <c r="P77" t="str">
+        <f t="shared" si="11"/>
+        <v>INSERT INTO `codesign_production`.`idea_project` (`idea_id`, `project_id`) VALUES (55, 20);</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Text too long" sqref="C7:C1048576 D2 C1">
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Text too long" sqref="C1 D2 C71:C1048576 C7:C67">
       <formula1>200</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>